<commit_message>
Update presentation, lower bounds data
Update presentation, lower bounds data
</commit_message>
<xml_diff>
--- a/LBs.xlsx
+++ b/LBs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>u_c_hihi_512_16.txt</t>
   </si>
@@ -33,9 +33,6 @@
     <t>11,0,0,0,0,7,0,3,1,1,0,0,7,2,6,0,3,3,2,3,4,14,0,3,0,9,0,0,10,4,7,0,0,0,2,3,9,12,5,0,0,13,6,2,3,5,2,7,4,0,7,5,1,10,0,2,13,4,4,3,4,5,0,2,0,0,0,2,5,0,1,0,11,3,4,0,0,14,2,8,0,9,12,3,0,0,4,0,2,1,0,0,0,0,11,0,0,2,2,0,2,4,0,0,1,0,12,0,0,12,0,4,2,2,2,0,0,7,1,9,2,2,11,8,1,6,0,1,0,1,1,7,4,10,3,8,0,0,8,6,1,11,11,7,12,10,0,0,11,3,1,15,0,0,12,4,2,0,1,12,14,0,8,1,1,6,2,13,0,0,4,5,2,1,1,3,0,3,13,12,6,1,0,0,15,0,0,5,5,0,5,10,0,2,10,5,5,2,3,2,8,2,11,0,9,1,8,6,1,1,0,1,2,5,0,1,3,8,8,0,0,5,1,13,0,1,5,0,5,3,6,0,6,1,0,0,8,1,0,5,1,0,0,0,14,0,7,8,1,1,11,10,6,1,0,0,0,0,1,2,0,6,0,3,1,0,9,4,7,13,0,0,1,1,6,0,0,0,1,15,6,0,0,0,8,0,2,2,0,10,15,14,0,0,0,1,0,1,0,11,0,0,0,0,0,6,0,0,12,12,6,0,0,1,2,0,0,0,1,0,0,0,2,2,8,1,0,11,0,0,0,13,1,10,0,9,1,2,5,1,1,0,8,1,7,0,10,0,0,0,0,0,1,0,2,0,11,0,5,5,2,8,3,6,0,0,5,3,7,5,2,5,1,6,0,6,1,12,1,1,1,0,1,4,0,10,0,0,1,0,11,14,2,0,0,2,10,2,2,1,1,15,4,0,1,2,8,3,13,15,0,2,9,4,8,0,10,3,3,2,11,4,9,3,3,3,0,1,0,0,0,2,2,9,10,1,5,6,0,2,4,4,1,0,0,10,0,3,11,0,10,5,0,7,0,1,2,4,3,1,14,0,2,2,6,0,0,9,0,0,5,4,0,0,3,7,1,14,0,1,0,1,0,3,2,15,1,5,7,6,0,3,14,11,3,0,13,0,3,2,13,0,0,6,8,4,0,0,0,1,6,2,</t>
   </si>
   <si>
-    <t>Chromosone</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -72,22 +69,55 @@
     <t>14,7,0,2,15,7,9,2,0,2,1,8,3,9,9,0,9,13,8,10,11,2,15,3,3,0,5,11,0,1,15,11,0,0,7,15,0,7,0,15,13,4,8,0,3,4,6,6,1,2,13,7,7,9,2,3,10,3,9,0,3,0,4,5,5,9,13,7,7,2,0,1,0,3,13,8,1,11,11,0,5,5,7,2,0,3,5,5,13,0,7,2,7,1,3,2,13,1,13,13,15,11,9,2,5,5,3,10,13,7,15,0,10,3,11,0,8,11,9,5,3,8,12,0,15,2,11,15,5,15,11,1,9,11,2,9,0,15,13,0,15,1,13,7,3,11,9,11,11,13,4,15,2,5,0,5,5,13,0,0,7,14,7,1,15,2,3,3,5,7,9,13,13,0,9,3,0,15,15,15,13,15,11,15,0,6,7,0,10,7,0,0,1,0,13,4,3,12,2,2,4,12,3,13,0,2,2,14,0,15,0,0,6,0,0,0,0,5,2,4,2,1,0,9,0,7,2,0,5,5,9,0,0,15,7,15,9,9,11,0,13,12,3,3,2,2,9,9,2,12,1,15,9,7,2,15,13,4,9,0,15,14,3,5,13,0,11,9,0,4,15,13,0,1,11,2,6,14,0,7,1,11,2,12,12,1,0,11,0,14,15,1,2,15,5,7,13,8,5,0,13,0,3,0,11,1,1,10,13,3,0,9,0,0,11,15,11,0,9,0,12,11,0,13,0,11,6,11,10,3,9,5,11,0,11,13,0,8,9,13,15,11,0,2,11,9,15,11,3,0,0,7,0,10,3,3,0,0,0,13,0,9,15,8,0,15,8,7,13,3,11,6,4,0,8,0,13,3,13,13,1,1,14,7,0,11,9,2,13,0,0,13,3,4,5,13,2,2,6,10,2,5,6,1,15,9,7,9,15,5,0,3,13,0,15,5,13,0,13,15,13,5,13,11,7,15,9,7,2,5,7,8,0,11,15,3,3,0,15,11,4,11,15,13,11,6,6,12,2,13,0,0,11,15,13,0,2,1,2,0,4,13,9,7,3,7,6,9,0,11,14,9,13,1,0,2,3,7,0,13,2,15,0,1,13,13,8,0,1,9,7,5,15,1,3,3,2,15,11,4,3,5,0,15,9,0,6,7,15,0,2,0,</t>
   </si>
   <si>
-    <t>Obs</t>
-  </si>
-  <si>
-    <t>MAX_ISTEPS 1000000000, pc=1.0, pm=0.009765625, popsize=512</t>
-  </si>
-  <si>
-    <t>MAX_ISTEPS 1000000000, pc=1.0, pm=0.009765625, popsize=1024:</t>
-  </si>
-  <si>
-    <t>MAX_ISTEPS 1000000000, pc=1.0, pm=0.009765625, popsize=1024</t>
-  </si>
-  <si>
-    <t>MAX_ISTEPS 1000000000, pc=1.0, pm=0.001953125, popsize=1024</t>
-  </si>
-  <si>
-    <t>MAX_ISTEPS 1000000000, pc=1.0, pm=0.009765625, popsize=2048</t>
+    <t>u_i_lohi_512_16.txt</t>
+  </si>
+  <si>
+    <t>10,0,7,0,7,9,13,12,8,4,6,13,4,5,5,4,5,13,6,10,3,1,8,11,8,4,10,5,9,13,11,0,5,13,2,7,8,4,11,4,6,4,11,6,15,4,3,7,2,12,12,12,12,11,2,2,3,6,1,6,14,6,3,5,4,4,11,14,6,15,3,10,7,8,11,4,6,1,0,4,9,12,7,1,2,3,8,12,7,10,6,8,8,13,5,3,15,1,14,5,6,11,14,0,10,7,7,3,0,11,5,5,8,4,8,9,10,1,5,6,0,3,2,0,0,0,5,0,3,2,13,12,14,5,0,6,6,9,4,2,0,0,13,4,6,9,1,5,15,0,10,0,9,8,5,2,0,15,15,8,4,7,14,12,3,1,13,14,10,14,14,12,3,11,9,8,1,15,8,13,15,14,6,12,13,7,10,7,2,10,15,11,15,1,5,14,3,6,8,8,2,0,2,10,8,10,6,13,1,1,13,15,15,9,15,12,12,1,13,13,9,15,8,5,10,0,5,13,1,15,2,11,9,0,0,6,9,3,11,14,1,5,10,15,12,5,7,6,15,3,8,11,10,13,4,9,0,13,9,6,9,13,8,5,6,13,3,9,0,4,14,1,2,14,4,3,8,3,14,9,9,15,2,8,10,0,13,14,12,9,0,3,10,11,1,14,11,8,7,14,7,6,4,13,15,0,5,4,8,12,1,11,12,12,13,13,12,11,7,7,6,9,13,1,6,1,15,9,9,3,14,14,11,5,13,3,10,6,2,15,8,3,0,15,14,11,0,14,11,13,11,2,8,13,9,13,12,15,13,7,9,12,8,15,1,6,13,8,11,9,2,12,14,15,15,8,7,5,9,0,6,3,5,9,4,3,5,13,15,11,7,3,8,15,12,8,4,11,2,15,13,5,8,12,8,8,13,11,0,10,12,5,7,2,15,13,0,8,15,9,6,3,10,13,13,9,2,13,6,2,8,9,5,4,2,13,5,13,0,6,3,11,13,9,8,9,3,9,13,1,9,11,15,2,5,1,13,4,1,5,13,4,11,12,1,15,0,10,5,5,2,9,1,15,11,10,8,1,12,11,9,12,0,4,14,15,0,2,2,3,5,4,14,10,8,12,6,13,5,10,4,8,13,10,4,6,1,2,2,14,3,0,</t>
+  </si>
+  <si>
+    <t>u_i_hilo_512_16.txt</t>
+  </si>
+  <si>
+    <t>3,5,2,13,3,6,3,8,13,15,7,4,1,5,6,8,14,5,13,2,9,1,11,3,3,4,3,11,4,15,1,5,15,1,10,0,4,7,10,12,9,11,3,11,5,2,14,7,8,4,5,10,14,11,13,0,14,2,9,0,7,9,9,6,9,8,15,8,9,12,6,4,15,5,14,9,9,2,9,2,5,9,4,2,4,10,3,10,14,11,4,6,2,5,3,7,2,5,14,15,8,1,10,2,6,0,2,12,2,5,4,12,1,8,6,13,9,4,9,7,12,8,1,12,0,10,11,8,12,9,5,13,4,0,14,5,12,13,6,4,10,2,14,3,7,3,0,8,12,1,7,13,2,1,4,0,10,2,12,9,10,14,2,0,10,2,0,3,5,13,0,11,5,0,1,4,10,5,6,12,6,10,12,2,5,11,0,6,9,8,2,7,11,8,1,14,9,5,11,9,15,13,4,13,6,6,5,13,10,12,9,8,3,9,0,10,12,5,15,8,7,9,10,11,14,9,0,5,4,1,2,13,6,12,11,11,0,0,6,4,7,9,9,10,2,7,10,14,13,13,14,6,0,2,5,13,13,13,8,14,8,15,6,8,9,14,4,13,10,14,13,7,4,6,15,7,12,9,6,15,10,1,13,7,7,0,10,5,15,5,15,8,12,8,1,10,1,13,9,14,11,11,12,14,6,12,5,0,15,11,1,6,13,13,12,12,4,11,9,15,8,3,10,7,5,0,6,8,1,1,12,6,14,14,6,1,9,12,13,11,2,13,3,0,11,13,14,15,4,9,10,9,1,4,11,7,11,9,6,11,7,5,14,10,4,5,4,10,3,4,10,2,10,7,13,10,13,4,1,12,5,12,6,7,10,5,2,1,12,13,8,0,1,14,0,1,10,13,14,7,13,13,1,13,4,8,8,6,10,9,5,3,11,14,10,3,15,10,13,15,8,9,3,6,2,10,8,2,15,1,6,2,10,4,6,7,2,3,2,14,3,9,2,12,7,7,2,2,4,11,2,8,9,14,6,10,0,0,15,15,5,2,2,14,9,12,7,1,1,9,3,14,12,13,12,0,13,9,10,9,13,3,3,4,13,5,11,3,10,8,15,11,15,9,11,1,9,8,1,0,2,7,13,8,7,4,12,9,12,14,3,1,</t>
+  </si>
+  <si>
+    <t>u_i_hihi_512_16.txt</t>
+  </si>
+  <si>
+    <t>9,10,11,11,2,7,12,15,7,15,2,7,15,9,8,14,15,15,0,4,14,10,4,5,1,6,13,11,11,2,5,11,10,6,6,14,1,11,14,4,5,5,6,13,0,9,0,7,0,13,11,10,0,6,15,8,11,5,2,11,9,13,11,2,9,8,7,15,14,11,5,2,0,8,3,10,12,10,1,2,12,13,0,15,0,2,9,1,10,4,12,7,13,6,5,2,4,11,4,14,1,8,10,4,6,0,10,2,5,11,15,10,0,5,15,13,13,4,15,6,8,1,15,1,4,8,5,11,0,4,13,10,9,14,1,6,4,1,15,5,1,4,1,11,4,12,1,2,5,2,10,1,10,2,13,5,9,7,12,14,7,2,4,2,8,6,4,5,2,5,11,7,4,10,1,3,3,0,9,15,5,9,7,13,8,1,11,7,9,9,14,0,0,8,5,0,12,5,8,8,9,12,15,12,0,13,10,0,4,4,5,2,6,2,6,15,7,3,10,14,4,5,11,7,15,1,9,15,8,15,12,9,6,7,13,14,4,9,13,8,7,15,10,15,4,8,15,14,1,10,12,5,12,4,6,2,14,13,6,6,2,11,7,7,5,3,11,7,0,15,0,8,6,1,0,12,7,9,10,11,5,15,6,2,9,6,6,9,15,15,6,12,11,13,12,7,6,5,15,4,0,9,15,14,2,0,9,14,14,8,13,1,4,13,11,6,0,11,5,11,6,12,6,11,4,11,11,13,13,0,6,9,6,12,8,2,0,5,8,14,1,8,0,12,1,15,15,5,5,6,5,3,2,0,5,1,8,6,12,3,12,4,12,6,9,2,9,13,6,13,11,6,5,6,11,8,13,15,12,6,8,14,8,15,3,8,6,5,13,0,2,14,5,11,1,14,4,0,10,11,15,8,7,13,1,11,4,0,7,6,14,4,14,13,13,12,4,10,9,4,5,11,0,0,4,8,9,11,14,12,3,7,14,9,11,6,3,8,10,9,11,5,15,15,14,4,2,0,2,7,5,1,6,5,3,12,6,14,3,7,3,12,12,2,8,2,14,6,4,9,5,11,10,13,11,4,6,11,9,5,5,0,4,12,13,7,11,11,12,5,11,8,15,11,13,9,6,0,4,6,8,9,12,12,10,14,14,8,1,5,2,9,</t>
+  </si>
+  <si>
+    <t>u_s_lolo_512_16.txt</t>
+  </si>
+  <si>
+    <t>5,4,9,6,15,15,5,15,2,3,1,13,11,2,10,6,5,0,9,9,9,12,12,5,0,3,0,2,12,2,15,5,11,9,9,13,15,3,12,15,7,11,2,3,13,7,1,15,15,0,14,4,15,15,5,14,1,2,7,12,7,4,4,11,2,12,15,14,11,6,12,0,0,1,3,13,10,10,6,8,1,3,1,4,5,0,15,1,5,13,9,7,12,5,6,1,9,8,14,1,1,0,8,15,7,0,0,3,5,7,11,15,13,5,2,9,5,15,15,10,1,6,7,9,15,7,8,13,11,7,12,1,15,1,7,2,13,15,13,11,12,8,13,5,13,9,7,12,6,0,3,0,12,0,14,0,0,4,11,5,11,5,11,5,9,11,0,1,5,9,1,2,1,13,0,0,6,5,3,1,3,6,10,13,3,15,13,15,8,3,12,9,7,13,1,12,2,5,2,11,2,3,9,10,5,0,3,3,8,1,8,13,3,4,3,7,11,15,8,10,15,1,0,6,5,4,7,0,0,9,7,4,0,7,1,1,9,7,3,11,8,9,8,8,4,9,4,3,15,3,9,10,8,0,7,7,2,11,1,13,6,9,11,13,0,11,11,4,0,4,2,1,7,3,0,13,13,14,0,10,1,6,2,0,11,13,5,2,3,7,11,3,3,6,15,7,3,12,7,2,3,6,1,4,5,7,14,10,10,5,9,7,2,12,6,0,2,13,1,1,4,0,11,1,10,11,9,9,13,5,13,0,15,0,9,15,11,5,8,11,10,0,6,11,11,2,14,0,9,4,2,6,10,15,3,1,13,4,13,2,8,2,3,13,0,3,7,1,0,12,3,11,4,11,2,13,4,0,4,6,0,2,15,8,6,0,15,5,9,11,13,12,9,11,0,5,13,13,6,13,3,7,3,9,9,11,5,15,4,1,9,11,10,13,15,3,0,7,1,13,4,8,8,8,0,6,0,1,8,4,7,15,1,1,4,1,3,11,9,0,9,0,1,6,4,2,9,0,0,0,3,13,2,14,6,12,13,4,6,2,10,11,3,8,8,1,4,2,13,9,14,6,7,7,13,15,4,2,8,15,10,8,13,15,0,0,4,8,5,3,1,6,0,7,0,2,12,11,8,0,7,3,4,9,1,4,14,13,11,6,5,15,</t>
+  </si>
+  <si>
+    <t>u_c_lohi_512_16.txt</t>
+  </si>
+  <si>
+    <t>15,0,1,0,12,0,7,0,0,14,1,9,1,3,7,1,12,7,0,0,3,8,0,1,15,0,1,0,3,0,0,0,10,11,9,0,0,0,0,5,0,0,0,11,3,8,1,0,14,2,1,0,2,1,0,0,1,5,3,0,1,3,11,10,1,1,1,13,0,4,15,2,8,8,0,6,11,0,1,0,0,4,0,3,6,0,1,0,4,0,0,1,0,0,2,0,13,4,1,12,0,4,6,11,0,1,0,1,15,8,1,1,1,0,0,0,0,6,3,1,13,0,0,0,0,2,8,1,5,3,2,2,0,0,1,0,9,2,8,12,13,0,0,2,12,2,0,4,4,1,0,2,2,0,10,0,0,0,1,1,2,7,8,2,0,15,0,15,4,0,0,0,6,3,5,1,0,0,11,5,1,2,0,2,3,11,4,0,5,3,0,0,4,0,4,2,10,0,1,3,0,0,2,9,1,2,1,5,0,0,1,0,5,0,7,0,7,0,0,1,3,0,0,9,0,0,0,8,5,0,0,0,5,0,1,0,9,13,1,8,14,0,5,0,0,0,8,7,0,3,4,2,12,1,8,3,0,14,15,9,15,15,0,11,4,5,6,1,0,6,1,0,2,2,1,8,0,5,8,10,0,5,3,2,8,0,6,0,4,10,11,15,0,11,1,0,3,3,0,1,7,0,0,11,13,1,2,9,0,7,1,0,12,9,1,0,3,14,5,12,1,3,0,0,2,0,0,1,4,11,1,8,0,7,5,1,0,0,0,2,2,0,5,0,4,0,0,3,11,0,10,1,3,15,2,0,1,1,1,3,0,10,2,0,3,0,12,15,14,12,0,0,0,4,0,0,0,0,0,2,3,14,0,0,1,5,0,1,2,7,0,1,2,7,1,0,0,1,0,11,14,5,10,15,0,0,4,12,3,7,1,3,2,1,0,2,0,6,2,0,0,2,0,12,4,1,0,3,3,6,12,0,2,0,7,12,0,0,4,6,1,0,0,3,0,1,1,7,1,0,11,4,0,8,13,0,14,0,14,4,0,0,9,1,0,1,1,9,0,3,1,0,0,3,6,1,9,3,2,5,1,5,10,0,3,7,0,2,6,0,2,14,0,0,9,0,6,9,4,15,4,3,3,6,0,4,0,0,0,0,2,0,</t>
+  </si>
+  <si>
+    <t>u_c_hilo_512_16.txt</t>
+  </si>
+  <si>
+    <t>11,5,0,11,13,0,7,1,2,12,5,7,6,10,0,0,0,6,12,1,5,2,11,2,1,5,3,10,0,8,3,15,5,0,14,0,0,8,2,1,13,7,11,3,12,8,1,10,4,9,0,1,0,2,3,8,3,0,4,0,0,0,2,2,1,6,12,0,4,1,8,5,2,6,4,8,1,11,4,11,1,2,14,14,0,0,4,0,14,11,7,9,10,8,7,7,4,0,5,3,5,0,1,13,4,2,3,2,6,4,7,2,14,4,7,11,1,3,0,13,13,15,13,0,4,6,12,5,4,1,10,1,15,2,14,7,9,8,9,7,5,4,5,9,3,14,1,10,13,13,13,0,6,9,2,4,5,3,7,2,6,1,6,1,5,2,3,0,1,1,15,5,1,5,6,1,0,3,1,7,13,10,14,0,4,3,8,8,0,5,6,5,10,13,1,13,0,5,5,0,6,6,5,8,11,1,9,1,1,1,1,1,1,5,12,10,9,11,6,12,0,1,14,3,9,15,14,15,2,6,0,0,13,10,6,0,11,1,7,1,3,9,1,12,8,2,13,4,0,0,1,12,15,2,4,1,1,12,1,5,3,2,2,1,10,3,7,1,0,2,7,9,15,0,6,1,0,0,12,7,5,15,13,2,14,4,2,1,10,8,5,6,2,1,0,0,9,0,6,5,13,3,0,8,0,2,14,10,1,0,2,3,11,2,3,2,13,2,4,2,3,3,3,3,2,1,4,11,5,5,5,0,1,0,2,8,1,0,4,5,9,9,1,7,9,9,1,8,13,11,4,0,6,13,2,3,2,14,3,10,0,12,15,5,11,11,5,0,0,0,1,7,4,0,2,1,12,3,4,0,0,12,10,3,5,8,14,0,3,7,3,7,0,14,2,1,1,0,6,6,1,5,1,0,0,4,5,4,0,8,8,2,0,0,8,1,10,4,2,1,2,1,14,2,12,3,15,2,14,15,4,3,12,2,4,0,4,0,14,8,10,12,3,1,9,5,1,5,1,2,4,4,0,12,6,7,14,8,3,2,11,5,0,1,7,4,2,1,1,5,10,1,15,8,2,14,3,1,0,3,1,1,4,4,8,1,5,0,5,13,7,5,1,9,12,13,7,0,1,7,1,9,1,15,4,1,0,5,3,2,3,3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Chromosone</t>
+  </si>
+  <si>
+    <t>Obs - STEPS 1000000000</t>
+  </si>
+  <si>
+    <t>pc=1.0, pm=5/512, popsize=2048</t>
+  </si>
+  <si>
+    <t>pc=1.0, pm=5/512, popsize=512</t>
+  </si>
+  <si>
+    <t>pc=1.0, pm=5/512, popsize=1024</t>
   </si>
 </sst>
 </file>
@@ -124,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -218,6 +248,28 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -229,11 +281,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -241,8 +290,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -254,6 +301,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,239 +621,324 @@
   <dimension ref="A1:DA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F13" sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="6" max="6" width="55.5546875" customWidth="1"/>
-    <col min="7" max="7" width="206.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="206.109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="72.6640625" style="2" customWidth="1"/>
-    <col min="10" max="105" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="206.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="206.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="72.6640625" style="1" customWidth="1"/>
+    <col min="10" max="105" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="F1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>7346524</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>8478411</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <f>(C2-B2)/B2</f>
         <v>0.1540710953915076</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="17">
+        <f>AVERAGE(D2:D5)</f>
+        <v>0.1160994344163141</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="e">
-        <f t="shared" ref="D3:D12" si="0">(C3-B3)/B3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="14"/>
+      <c r="A3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6">
+        <v>152700</v>
+      </c>
+      <c r="C3" s="6">
+        <v>167048</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">(C3-B3)/B3</f>
+        <v>9.3962017026850031E-2</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="e">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="6">
+        <v>238138</v>
+      </c>
+      <c r="C4" s="6">
+        <v>270916</v>
+      </c>
+      <c r="D4" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="14"/>
+        <v>0.13764287933887073</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="A5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
         <v>5132</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>5536</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <f t="shared" si="0"/>
         <v>7.8721745908028065E-2</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2909326</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3505029</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.20475635937670786</v>
+      </c>
+      <c r="E6" s="17">
+        <f>AVERAGE(D6:D9)</f>
+        <v>0.24070089049042478</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="13">
+        <v>73057</v>
+      </c>
+      <c r="C7" s="6">
+        <v>90416</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23760899024049714</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="e">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13">
+        <v>101063</v>
+      </c>
+      <c r="C8" s="6">
+        <v>135997</v>
+      </c>
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14"/>
+        <v>0.34566557493840477</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
         <v>2529</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>2971</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>0.17477263740608937</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
+      <c r="E9" s="19"/>
+      <c r="F9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
         <v>4063563</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>5009057</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <f t="shared" si="0"/>
         <v>0.23267610222851226</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
+      <c r="E10" s="17">
+        <f>AVERAGE(D10:D13)</f>
+        <v>0.20110584028795492</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="7">
+      <c r="A11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
         <v>95419</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>110505</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f t="shared" si="0"/>
         <v>0.15810268395183349</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>16</v>
+      <c r="E11" s="18"/>
+      <c r="F11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="7">
+      <c r="A12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
         <v>120452</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>151330</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>0.25635107760767772</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="15"/>
+      <c r="B13" s="3">
+        <v>3414</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3951</v>
+      </c>
+      <c r="D13" s="14">
+        <f t="shared" si="0"/>
+        <v>0.15729349736379614</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>